<commit_message>
Replace audio files with updated versions
</commit_message>
<xml_diff>
--- a/Assets/Audio/list.xlsx
+++ b/Assets/Audio/list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\TGC-Jam-NameTBD\Assets\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6B4862-FDDA-4304-90F5-667EB30C822D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9256468-1487-418C-9773-37517429143E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10290" yWindow="5565" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25050" yWindow="7755" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Interaction</t>
   </si>
@@ -69,9 +69,6 @@
     <t>背景人声</t>
   </si>
   <si>
-    <t>voice1.mp3//voice2.mp3</t>
-  </si>
-  <si>
     <t>IF RED</t>
   </si>
   <si>
@@ -106,6 +103,15 @@
   </si>
   <si>
     <t>太空背景音.mp3//监控室声音.mp3</t>
+  </si>
+  <si>
+    <t>Invalid Click 2</t>
+  </si>
+  <si>
+    <t>invalid_click_2.mp3</t>
+  </si>
+  <si>
+    <t>voice_1.mp3//voice_2.mp3</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -475,7 +481,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -486,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -497,7 +503,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,7 +514,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,65 +522,76 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>